<commit_message>
Test concluant, version du déploiement uniquement sur modification du xlsx validée
</commit_message>
<xml_diff>
--- a/source/requirements_app_PEGS.xlsx
+++ b/source/requirements_app_PEGS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Etu\Desktop\M2\S2\Requierments\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765857CA-2F0E-4778-8328-D9327C067C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C5AE89-3EFB-474D-8EBE-6CBB9B9450D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="318">
   <si>
     <t>ID</t>
   </si>
@@ -979,15 +979,6 @@
   </si>
   <si>
     <t>Protège le Time-to-Code et évite de s'éparpiller</t>
-  </si>
-  <si>
-    <t>S-63</t>
-  </si>
-  <si>
-    <t>S.7</t>
-  </si>
-  <si>
-    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -1153,8 +1144,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02395E64-223E-4C7E-B1E7-DFD1E0F05F91}" name="Tableau1" displayName="Tableau1" ref="A1:N50" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:N50" xr:uid="{02395E64-223E-4C7E-B1E7-DFD1E0F05F91}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02395E64-223E-4C7E-B1E7-DFD1E0F05F91}" name="Tableau1" displayName="Tableau1" ref="A1:N49" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:N49" xr:uid="{02395E64-223E-4C7E-B1E7-DFD1E0F05F91}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{FED874BB-E7AB-4992-B9CF-6CB8848E8D74}" name="#" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{C2490B20-ACE7-4EE7-9C1C-FFF1C4CD6777}" name="ID" dataDxfId="11"/>
@@ -1460,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3639,50 +3630,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="3">
-        <v>49</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="I50" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="L50" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="M50" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="N50" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>